<commit_message>
Scorecard knowledge: add shortcut name
</commit_message>
<xml_diff>
--- a/lib/csc_core/samples/assets/csv/scorecard_knowledges.xlsx
+++ b/lib/csc_core/samples/assets/csv/scorecard_knowledges.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/www/csc-web/lib/samples/assets/csv/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14380" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="ScorecardKnowledge" sheetId="1" r:id="rId4"/>
+    <sheet name="ScorecardKnowledge" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>code</t>
   </si>
@@ -25,12 +41,6 @@
     <t>sk_001</t>
   </si>
   <si>
-    <t>មេរៀនម៉ូឌុលទី ១- ការណែនាំអំពីគណនេយ្យភាពសង្គម (ISAF)</t>
-  </si>
-  <si>
-    <t>Module 1- introduction to ISAF</t>
-  </si>
-  <si>
     <t>sk_002</t>
   </si>
   <si>
@@ -46,9 +56,6 @@
     <t>មេរៀនម៉ូឌុលទី ៣៖ ការសម្របសម្រួលប័ណ្ណដាក់ពិន្ទុសហគមន៍ (CSC) និង ការវាយតម្លៃខ្លួនឯងដោយអ្នកផ្តល់សេវា (SSA)</t>
   </si>
   <si>
-    <t>Module3: Facilitating community scorecard and service provider self-assessment</t>
-  </si>
-  <si>
     <t>sk_004</t>
   </si>
   <si>
@@ -56,42 +63,91 @@
   </si>
   <si>
     <t>Module 4: Facilitating the interface meeting and JAAP.</t>
+  </si>
+  <si>
+    <t>Module 3: Facilitating community scorecard and service provider self-assessment</t>
+  </si>
+  <si>
+    <t>shortcut_name_km</t>
+  </si>
+  <si>
+    <t>shortcut_name_en</t>
+  </si>
+  <si>
+    <t>មេរៀនម៉ូឌុលទី ១</t>
+  </si>
+  <si>
+    <t>Module 1</t>
+  </si>
+  <si>
+    <t>Module 2</t>
+  </si>
+  <si>
+    <t>Module 3</t>
+  </si>
+  <si>
+    <t>Module 4</t>
+  </si>
+  <si>
+    <t>មេរៀនម៉ូឌុលទី ២</t>
+  </si>
+  <si>
+    <t>មេរៀនម៉ូឌុលទី ៣</t>
+  </si>
+  <si>
+    <t>មេរៀនម៉ូឌុលទី ៤</t>
+  </si>
+  <si>
+    <t>Module 1: introduction to ISAF</t>
+  </si>
+  <si>
+    <t>មេរៀនម៉ូឌុលទី ១៖ ការណែនាំអំពីគណនេយ្យភាពសង្គម (ISAF)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="&quot;Khmer OS Battambang&quot;"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -100,7 +156,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -110,46 +166,47 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -339,20 +396,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="42.5" customWidth="1"/>
+    <col min="3" max="3" width="41.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -362,52 +429,82 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4">
-      <c r="A4" s="6" t="s">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>14</v>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>